<commit_message>
added hyperlinks into bug-report
</commit_message>
<xml_diff>
--- a/test game kkrieger/bug-report exaple.xlsx
+++ b/test game kkrieger/bug-report exaple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitrep\Portfolio\test game kkrieger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E601E8-1DFE-4F9B-A1A1-23CE07BBC4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A87991-293C-4C64-B74B-36AC8685FDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t xml:space="preserve">Applications </t>
   </si>
   <si>
-    <t>hanging projectiles</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bypassing the bug </t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t xml:space="preserve">Снаряд исчезнет </t>
+  </si>
+  <si>
+    <t>projectiles bug</t>
   </si>
 </sst>
 </file>
@@ -393,31 +393,88 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -425,63 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -767,7 +767,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:O7"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,321 +780,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14"/>
-      <c r="I1" s="24" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="I1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="26"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="5"/>
-      <c r="I2" s="21" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="6"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="1:15" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="I3" s="27" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="I3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28" t="s">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="29"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="I4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="9"/>
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="I5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="I6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="I7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="I8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="6"/>
-      <c r="I4" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="6"/>
-      <c r="I5" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="6"/>
-      <c r="I6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="6"/>
-      <c r="I7" s="21" t="s">
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="23"/>
+    </row>
+    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="I9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="I10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="I11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
-      <c r="I8" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="I9" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="I10" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="2" t="s">
+      <c r="J11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="5"/>
-      <c r="I11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="10"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="I12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="J12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="5"/>
-      <c r="I12" s="27" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="I13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="J13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-      <c r="I13" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="23"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="12"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B4:D7"/>
+    <mergeCell ref="E4:G7"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J1:O1"/>
     <mergeCell ref="J3:L3"/>
@@ -1102,24 +1109,19 @@
     <mergeCell ref="J8:O8"/>
     <mergeCell ref="J4:L7"/>
     <mergeCell ref="M4:O7"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B4:D7"/>
-    <mergeCell ref="E4:G7"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="J13:O13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="https://github.com/Zimancer/Portfolio" xr:uid="{D4F51733-FA4F-4CE7-9205-68ABB8EC09F0}"/>
     <hyperlink ref="B8:G8" r:id="rId2" display="зависающие снаряды" xr:uid="{040F2C73-4296-4FB2-917D-23607FA9E2F4}"/>
+    <hyperlink ref="J8" r:id="rId3" display="https://github.com/Zimancer/Portfolio" xr:uid="{6009C0E6-581F-49EB-B7D4-F29BBC2C2D76}"/>
+    <hyperlink ref="J8:O8" r:id="rId4" display="зависающие снаряды" xr:uid="{EE53427B-1FE9-4CFF-B291-A452F1FEBAFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>